<commit_message>
Cập nhật phân công
</commit_message>
<xml_diff>
--- a/Phân công thực hiện.xls.xlsx
+++ b/Phân công thực hiện.xls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Xây dựng phần mềm quản lý thư viện của Học viện Kỹ thuật Quân sự</t>
   </si>
@@ -32,102 +32,57 @@
     <t>Đặng Quốc Đạt</t>
   </si>
   <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>3.3</t>
-  </si>
-  <si>
     <t>Xây dựng module thêm,sửa,xóa đầu sách mới</t>
   </si>
   <si>
     <t>Nguyễn Đức Hạnh</t>
   </si>
   <si>
-    <t>3.4</t>
-  </si>
-  <si>
     <t>Xây dựng module tìm kiếm đầu sách</t>
   </si>
   <si>
-    <t>3.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Xây dựng module thêm,sửa,xóa độc giả </t>
   </si>
   <si>
     <t>Trương Phạm Dũng</t>
   </si>
   <si>
-    <t>3.6</t>
-  </si>
-  <si>
     <t>Xây dựng module tìm kiếm độc giả</t>
   </si>
   <si>
-    <t>3.7</t>
-  </si>
-  <si>
     <t>Xây dựng module thêm,sửa,xóa nhân viên thư viện</t>
   </si>
   <si>
     <t>Lê Minh Hiếu</t>
   </si>
   <si>
-    <t>3.8</t>
-  </si>
-  <si>
     <t>Xây dựng module tìm kiếm nhân viên thư viện</t>
   </si>
   <si>
-    <t>3.9</t>
-  </si>
-  <si>
     <t>Xây dựng module thêm,sửa,xóa người dùng</t>
   </si>
   <si>
     <t>Đỗ Tiến Đạt</t>
   </si>
   <si>
-    <t>3.10</t>
-  </si>
-  <si>
     <t>Xây dựng module tìm kiếm người dùng</t>
   </si>
   <si>
-    <t>3.11</t>
-  </si>
-  <si>
     <t>Xây dựng module quản lý thông tin mượn trả (thêm, sửa, xóa, tìm kiếm)</t>
   </si>
   <si>
     <t>Phạm Ngọc Dũng</t>
   </si>
   <si>
-    <t>3.12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Xây dựng module tìm kiếm thông tin mượn trả </t>
   </si>
   <si>
-    <t>3.13</t>
-  </si>
-  <si>
     <t>Xây dựng module đăng nhập,đăng ký</t>
   </si>
   <si>
-    <t>3.14</t>
-  </si>
-  <si>
     <t>Ghép nối các module để nhận được phần mềm hoàn chỉnh</t>
   </si>
   <si>
-    <t>3.15</t>
-  </si>
-  <si>
     <t>Chạy kiểm thử phần mềm kết quả</t>
   </si>
   <si>
@@ -150,6 +105,15 @@
   </si>
   <si>
     <t xml:space="preserve">           30/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xây dựng tài liệu hướng dẫn cài đặt, vận hành</t>
+  </si>
+  <si>
+    <t>Bonsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           29/10</t>
   </si>
 </sst>
 </file>
@@ -467,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,10 +446,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,213 +464,227 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3">
+        <v>3.1</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
+      <c r="B4">
+        <v>3.2</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>3.3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3.4</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3.5</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3.6</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3.7</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3.8</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3.9</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3.1</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3.11</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D13" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>3.12</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>3.13</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>31</v>
+      <c r="B16">
+        <v>3.14</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>33</v>
+      <c r="B17">
+        <v>3.15</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>3.16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update phân công lại cv nhé
</commit_message>
<xml_diff>
--- a/Phân công thực hiện.xls.xlsx
+++ b/Phân công thực hiện.xls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Xây dựng phần mềm quản lý thư viện của Học viện Kỹ thuật Quân sự</t>
   </si>
@@ -89,9 +89,6 @@
     <t xml:space="preserve">                                                                         Phân công công việc</t>
   </si>
   <si>
-    <t>Thiết kế giao diện cửa sổ chính (màn hình đăng nhập, các menu trỏ đến các module con,…).</t>
-  </si>
-  <si>
     <t>Xây dựng CSDL đầu sách, độc giả, thông tin mượn trả,nhân viên,người dùng</t>
   </si>
   <si>
@@ -107,13 +104,19 @@
     <t xml:space="preserve">           30/10</t>
   </si>
   <si>
-    <t xml:space="preserve"> Xây dựng tài liệu hướng dẫn cài đặt, vận hành</t>
-  </si>
-  <si>
-    <t>Bonsi</t>
-  </si>
-  <si>
     <t xml:space="preserve">           29/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Xây dựng tài liệu hướng dẫn cài đặt, vận hành </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonsi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           21/10</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện cửa sổ chính (màn hình đăng nhập, các menu trỏ đến các module con,…),phân công cv</t>
   </si>
 </sst>
 </file>
@@ -434,12 +437,12 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="94.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
@@ -449,7 +452,7 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -468,13 +471,13 @@
         <v>3.1</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -482,13 +485,13 @@
         <v>3.2</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -502,7 +505,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -516,7 +519,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -530,7 +533,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -544,7 +547,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,7 +561,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -572,7 +575,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -600,7 +603,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -614,7 +617,7 @@
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -628,7 +631,7 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -664,13 +667,13 @@
         <v>3.15</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -678,13 +681,13 @@
         <v>3.16</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ae làm theo kiểu Linq to SQL để kết nối đến CSDL nhé
</commit_message>
<xml_diff>
--- a/Phân công thực hiện.xls.xlsx
+++ b/Phân công thực hiện.xls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Xây dựng phần mềm quản lý thư viện của Học viện Kỹ thuật Quân sự</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Thiết kế giao diện cửa sổ chính (màn hình đăng nhập, các menu trỏ đến các module con,…),phân công cv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +693,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Phân công cv update
</commit_message>
<xml_diff>
--- a/Phân công thực hiện.xls.xlsx
+++ b/Phân công thực hiện.xls.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +561,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
@@ -575,7 +575,7 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -589,7 +589,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -603,7 +603,7 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Phân công update lần cuối
</commit_message>
<xml_diff>
--- a/Phân công thực hiện.xls.xlsx
+++ b/Phân công thực hiện.xls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Xây dựng phần mềm quản lý thư viện của Học viện Kỹ thuật Quân sự</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Xây dựng module thêm,sửa,xóa,tìm kiếm nhà xuất bản</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +648,7 @@
         <v>3.13</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -659,13 +662,13 @@
         <v>3.14</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -673,13 +676,13 @@
         <v>3.15</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -687,22 +690,36 @@
         <v>3.16</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>3.17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
       <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>